<commit_message>
added cytology (fixed) to valid sources
</commit_message>
<xml_diff>
--- a/tests/fixtures/orderforms/1508.35.balsamic.xlsx
+++ b/tests/fixtures/orderforms/1508.35.balsamic.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jsdiazboada/Documents/Clinical_Genomics/repos/cg/tests/fixtures/orderforms/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AC62AAE-EDBB-864C-91FD-F6E1F9324F25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59B70CD1-D6BE-5D4B-99AC-CF36AE8108AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="59080" yWindow="-13500" windowWidth="29880" windowHeight="33360" tabRatio="993" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28800" yWindow="-13500" windowWidth="60160" windowHeight="33360" tabRatio="993" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Information" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1336" uniqueCount="836">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1337" uniqueCount="837">
   <si>
     <t>https://clinical.scilifelab.se/</t>
   </si>
@@ -3774,6 +3774,9 @@
   </si>
   <si>
     <t>GMCKsolid</t>
+  </si>
+  <si>
+    <t>cytology (fixed)</t>
   </si>
 </sst>
 </file>
@@ -5970,8 +5973,8 @@
   </sheetPr>
   <dimension ref="A1:AMM395"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="Z4" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="Z15" sqref="Z15:Z56"/>
+    <sheetView showGridLines="0" topLeftCell="A4" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="I30" sqref="I30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" outlineLevelRow="1" x14ac:dyDescent="0.15"/>
@@ -28515,7 +28518,7 @@
         <v>67</v>
       </c>
       <c r="I30" s="82" t="s">
-        <v>133</v>
+        <v>836</v>
       </c>
       <c r="J30" s="83" t="s">
         <v>93</v>
@@ -71689,12 +71692,6 @@
           </x14:formula1>
           <xm:sqref>D15:D394</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{BE497A2B-81FE-9B4E-B96E-C607ADE86557}">
-          <x14:formula1>
-            <xm:f>'Drop-down lists'!$G$2:$G$21</xm:f>
-          </x14:formula1>
-          <xm:sqref>I15:I394</xm:sqref>
-        </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{64EB9F58-6FDA-8B4A-B5D0-278667DD507F}">
           <x14:formula1>
             <xm:f>'Drop-down lists'!$F$2:$F$209</xm:f>
@@ -71731,6 +71728,12 @@
           </x14:formula1>
           <xm:sqref>C15 C16:C17 C19:C394 C18</xm:sqref>
         </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{BE497A2B-81FE-9B4E-B96E-C607ADE86557}">
+          <x14:formula1>
+            <xm:f>'Drop-down lists'!$G$2:$G$22</xm:f>
+          </x14:formula1>
+          <xm:sqref>I15:I394</xm:sqref>
+        </x14:dataValidation>
       </x14:dataValidations>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
@@ -71744,8 +71747,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AL313"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -72158,7 +72161,7 @@
         <v>114</v>
       </c>
       <c r="G10" s="123" t="s">
-        <v>536</v>
+        <v>836</v>
       </c>
       <c r="M10" s="118" t="s">
         <v>116</v>
@@ -72182,7 +72185,7 @@
         <v>118</v>
       </c>
       <c r="G11" s="123" t="s">
-        <v>535</v>
+        <v>536</v>
       </c>
       <c r="M11" s="122" t="s">
         <v>120</v>
@@ -72204,8 +72207,8 @@
       <c r="F12" s="116" t="s">
         <v>123</v>
       </c>
-      <c r="G12" s="138" t="s">
-        <v>562</v>
+      <c r="G12" s="123" t="s">
+        <v>535</v>
       </c>
       <c r="M12" s="122" t="s">
         <v>125</v>
@@ -72228,8 +72231,8 @@
       <c r="F13" s="116" t="s">
         <v>128</v>
       </c>
-      <c r="G13" s="123" t="s">
-        <v>110</v>
+      <c r="G13" s="138" t="s">
+        <v>562</v>
       </c>
       <c r="M13" s="118" t="s">
         <v>130</v>
@@ -72252,8 +72255,8 @@
       <c r="F14" s="116" t="s">
         <v>132</v>
       </c>
-      <c r="G14" s="116" t="s">
-        <v>115</v>
+      <c r="G14" s="123" t="s">
+        <v>110</v>
       </c>
       <c r="M14" s="122" t="s">
         <v>134</v>
@@ -72278,7 +72281,7 @@
         <v>137</v>
       </c>
       <c r="G15" s="116" t="s">
-        <v>532</v>
+        <v>115</v>
       </c>
       <c r="M15" s="122" t="s">
         <v>139</v>
@@ -72303,7 +72306,7 @@
         <v>141</v>
       </c>
       <c r="G16" s="116" t="s">
-        <v>119</v>
+        <v>532</v>
       </c>
       <c r="M16" s="118" t="s">
         <v>142</v>
@@ -72328,7 +72331,7 @@
         <v>145</v>
       </c>
       <c r="G17" s="116" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="M17" s="122" t="s">
         <v>146</v>
@@ -72352,7 +72355,7 @@
         <v>148</v>
       </c>
       <c r="G18" s="116" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="M18" s="118" t="s">
         <v>149</v>
@@ -72376,7 +72379,7 @@
         <v>151</v>
       </c>
       <c r="G19" s="116" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="M19" s="122" t="s">
         <v>152</v>
@@ -72400,7 +72403,7 @@
         <v>154</v>
       </c>
       <c r="G20" s="116" t="s">
-        <v>533</v>
+        <v>133</v>
       </c>
       <c r="M20" s="122" t="s">
         <v>155</v>
@@ -72424,7 +72427,7 @@
         <v>157</v>
       </c>
       <c r="G21" s="116" t="s">
-        <v>138</v>
+        <v>533</v>
       </c>
       <c r="M21" s="118" t="s">
         <v>158</v>
@@ -72448,6 +72451,9 @@
       <c r="F22" s="116" t="s">
         <v>160</v>
       </c>
+      <c r="G22" s="116" t="s">
+        <v>138</v>
+      </c>
       <c r="M22" s="122" t="s">
         <v>161</v>
       </c>
@@ -72486,7 +72492,6 @@
       <c r="F24" s="116" t="s">
         <v>167</v>
       </c>
-      <c r="G24" s="126"/>
       <c r="M24" s="118" t="s">
         <v>168</v>
       </c>
@@ -72626,6 +72631,7 @@
       <c r="F31" s="116" t="s">
         <v>189</v>
       </c>
+      <c r="G31" s="126"/>
       <c r="M31" s="122" t="s">
         <v>190</v>
       </c>
@@ -74698,7 +74704,7 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="eJGU3TnrM7TUS36P6EF6OoUepfRxqvEYBttmdh2jpK/p0PFzl3txM9S88hoDVu8ScxrhCTA1475ID05WI3/y1w==" saltValue="ht+aVAqcEGcaWx2xT5yeQg==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="DOBEA5PPJ0/DO9fCp3Rawg7h486WafWIm9j5JEZC7y6BGeboIqOLe0uxZvxuUHdmH5ObXAfaHJRTYgEeq7v1Wg==" saltValue="NhKsolv4mAuZFOU4YMM8gg==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <phoneticPr fontId="41" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>